<commit_message>
Shopify Sample file update and Remove Anjun Dropdown
</commit_message>
<xml_diff>
--- a/public/uploads/shopify-format.xlsx
+++ b/public/uploads/shopify-format.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hd-v2\public\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\hd-v2\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA5A3D9-96F8-4420-AB4E-31BFA4ED4818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18540" windowHeight="5685"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -23,6 +24,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -203,7 +206,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -568,53 +571,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AF982"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M6" sqref="M6"/>
+      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="8.125" customWidth="1"/>
-    <col min="3" max="3" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.09765625" customWidth="1"/>
+    <col min="3" max="3" width="8.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.8984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.8984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.09765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.09765625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.8984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.19921875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.69921875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="22.69921875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.59765625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.8984375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.5" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="30" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.09765625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.59765625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,13 +709,13 @@
         <v>29</v>
       </c>
       <c r="AE1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" s="15" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:32" s="15" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>32</v>
       </c>
@@ -793,7 +796,7 @@
       <c r="AE2" s="9"/>
       <c r="AF2" s="9"/>
     </row>
-    <row r="3" spans="1:32" s="15" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" s="15" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>44</v>
       </c>
@@ -874,7 +877,7 @@
       <c r="AE3" s="16"/>
       <c r="AF3" s="16"/>
     </row>
-    <row r="4" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -908,7 +911,7 @@
       <c r="AE4" s="6"/>
       <c r="AF4" s="6"/>
     </row>
-    <row r="5" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -942,7 +945,7 @@
       <c r="AE5" s="6"/>
       <c r="AF5" s="6"/>
     </row>
-    <row r="6" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -976,7 +979,7 @@
       <c r="AE6" s="6"/>
       <c r="AF6" s="6"/>
     </row>
-    <row r="7" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1010,7 +1013,7 @@
       <c r="AE7" s="6"/>
       <c r="AF7" s="6"/>
     </row>
-    <row r="8" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1044,7 +1047,7 @@
       <c r="AE8" s="6"/>
       <c r="AF8" s="6"/>
     </row>
-    <row r="9" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1078,7 +1081,7 @@
       <c r="AE9" s="6"/>
       <c r="AF9" s="6"/>
     </row>
-    <row r="10" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1112,7 +1115,7 @@
       <c r="AE10" s="6"/>
       <c r="AF10" s="6"/>
     </row>
-    <row r="11" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1146,7 +1149,7 @@
       <c r="AE11" s="6"/>
       <c r="AF11" s="6"/>
     </row>
-    <row r="12" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1180,7 +1183,7 @@
       <c r="AE12" s="6"/>
       <c r="AF12" s="6"/>
     </row>
-    <row r="13" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1214,7 +1217,7 @@
       <c r="AE13" s="6"/>
       <c r="AF13" s="6"/>
     </row>
-    <row r="14" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1248,7 +1251,7 @@
       <c r="AE14" s="6"/>
       <c r="AF14" s="6"/>
     </row>
-    <row r="15" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1282,7 +1285,7 @@
       <c r="AE15" s="6"/>
       <c r="AF15" s="6"/>
     </row>
-    <row r="16" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1316,7 +1319,7 @@
       <c r="AE16" s="6"/>
       <c r="AF16" s="6"/>
     </row>
-    <row r="17" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1350,7 +1353,7 @@
       <c r="AE17" s="6"/>
       <c r="AF17" s="6"/>
     </row>
-    <row r="18" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1384,7 +1387,7 @@
       <c r="AE18" s="6"/>
       <c r="AF18" s="6"/>
     </row>
-    <row r="19" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1418,7 +1421,7 @@
       <c r="AE19" s="6"/>
       <c r="AF19" s="6"/>
     </row>
-    <row r="20" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1452,7 +1455,7 @@
       <c r="AE20" s="6"/>
       <c r="AF20" s="6"/>
     </row>
-    <row r="21" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1486,7 +1489,7 @@
       <c r="AE21" s="6"/>
       <c r="AF21" s="6"/>
     </row>
-    <row r="22" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1520,7 +1523,7 @@
       <c r="AE22" s="6"/>
       <c r="AF22" s="6"/>
     </row>
-    <row r="23" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1554,7 +1557,7 @@
       <c r="AE23" s="6"/>
       <c r="AF23" s="6"/>
     </row>
-    <row r="24" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1588,7 +1591,7 @@
       <c r="AE24" s="6"/>
       <c r="AF24" s="6"/>
     </row>
-    <row r="25" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1622,7 +1625,7 @@
       <c r="AE25" s="6"/>
       <c r="AF25" s="6"/>
     </row>
-    <row r="26" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1656,7 +1659,7 @@
       <c r="AE26" s="6"/>
       <c r="AF26" s="6"/>
     </row>
-    <row r="27" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1690,7 +1693,7 @@
       <c r="AE27" s="6"/>
       <c r="AF27" s="6"/>
     </row>
-    <row r="28" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1724,7 +1727,7 @@
       <c r="AE28" s="6"/>
       <c r="AF28" s="6"/>
     </row>
-    <row r="29" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1758,7 +1761,7 @@
       <c r="AE29" s="6"/>
       <c r="AF29" s="6"/>
     </row>
-    <row r="30" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1792,7 +1795,7 @@
       <c r="AE30" s="6"/>
       <c r="AF30" s="6"/>
     </row>
-    <row r="31" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -1826,7 +1829,7 @@
       <c r="AE31" s="6"/>
       <c r="AF31" s="6"/>
     </row>
-    <row r="32" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1860,7 +1863,7 @@
       <c r="AE32" s="6"/>
       <c r="AF32" s="6"/>
     </row>
-    <row r="33" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -1894,7 +1897,7 @@
       <c r="AE33" s="6"/>
       <c r="AF33" s="6"/>
     </row>
-    <row r="34" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -1928,7 +1931,7 @@
       <c r="AE34" s="6"/>
       <c r="AF34" s="6"/>
     </row>
-    <row r="35" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -1962,7 +1965,7 @@
       <c r="AE35" s="6"/>
       <c r="AF35" s="6"/>
     </row>
-    <row r="36" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1996,7 +1999,7 @@
       <c r="AE36" s="6"/>
       <c r="AF36" s="6"/>
     </row>
-    <row r="37" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -2030,7 +2033,7 @@
       <c r="AE37" s="6"/>
       <c r="AF37" s="6"/>
     </row>
-    <row r="38" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -2064,7 +2067,7 @@
       <c r="AE38" s="6"/>
       <c r="AF38" s="6"/>
     </row>
-    <row r="39" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -2098,7 +2101,7 @@
       <c r="AE39" s="6"/>
       <c r="AF39" s="6"/>
     </row>
-    <row r="40" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -2132,7 +2135,7 @@
       <c r="AE40" s="6"/>
       <c r="AF40" s="6"/>
     </row>
-    <row r="41" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -2166,7 +2169,7 @@
       <c r="AE41" s="6"/>
       <c r="AF41" s="6"/>
     </row>
-    <row r="42" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -2200,7 +2203,7 @@
       <c r="AE42" s="6"/>
       <c r="AF42" s="6"/>
     </row>
-    <row r="43" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -2234,7 +2237,7 @@
       <c r="AE43" s="6"/>
       <c r="AF43" s="6"/>
     </row>
-    <row r="44" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -2268,7 +2271,7 @@
       <c r="AE44" s="6"/>
       <c r="AF44" s="6"/>
     </row>
-    <row r="45" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -2302,7 +2305,7 @@
       <c r="AE45" s="6"/>
       <c r="AF45" s="6"/>
     </row>
-    <row r="46" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -2336,7 +2339,7 @@
       <c r="AE46" s="6"/>
       <c r="AF46" s="6"/>
     </row>
-    <row r="47" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -2370,7 +2373,7 @@
       <c r="AE47" s="6"/>
       <c r="AF47" s="6"/>
     </row>
-    <row r="48" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -2404,7 +2407,7 @@
       <c r="AE48" s="6"/>
       <c r="AF48" s="6"/>
     </row>
-    <row r="49" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -2438,7 +2441,7 @@
       <c r="AE49" s="6"/>
       <c r="AF49" s="6"/>
     </row>
-    <row r="50" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -2472,7 +2475,7 @@
       <c r="AE50" s="6"/>
       <c r="AF50" s="6"/>
     </row>
-    <row r="51" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -2506,7 +2509,7 @@
       <c r="AE51" s="6"/>
       <c r="AF51" s="6"/>
     </row>
-    <row r="52" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -2540,7 +2543,7 @@
       <c r="AE52" s="6"/>
       <c r="AF52" s="6"/>
     </row>
-    <row r="53" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -2574,7 +2577,7 @@
       <c r="AE53" s="6"/>
       <c r="AF53" s="6"/>
     </row>
-    <row r="54" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -2608,7 +2611,7 @@
       <c r="AE54" s="6"/>
       <c r="AF54" s="6"/>
     </row>
-    <row r="55" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -2642,7 +2645,7 @@
       <c r="AE55" s="6"/>
       <c r="AF55" s="6"/>
     </row>
-    <row r="56" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -2676,7 +2679,7 @@
       <c r="AE56" s="6"/>
       <c r="AF56" s="6"/>
     </row>
-    <row r="57" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -2710,7 +2713,7 @@
       <c r="AE57" s="6"/>
       <c r="AF57" s="6"/>
     </row>
-    <row r="58" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -2744,7 +2747,7 @@
       <c r="AE58" s="6"/>
       <c r="AF58" s="6"/>
     </row>
-    <row r="59" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -2778,7 +2781,7 @@
       <c r="AE59" s="6"/>
       <c r="AF59" s="6"/>
     </row>
-    <row r="60" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -2812,7 +2815,7 @@
       <c r="AE60" s="6"/>
       <c r="AF60" s="6"/>
     </row>
-    <row r="61" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -2846,7 +2849,7 @@
       <c r="AE61" s="6"/>
       <c r="AF61" s="6"/>
     </row>
-    <row r="62" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -2880,7 +2883,7 @@
       <c r="AE62" s="6"/>
       <c r="AF62" s="6"/>
     </row>
-    <row r="63" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -2914,7 +2917,7 @@
       <c r="AE63" s="6"/>
       <c r="AF63" s="6"/>
     </row>
-    <row r="64" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -2948,7 +2951,7 @@
       <c r="AE64" s="6"/>
       <c r="AF64" s="6"/>
     </row>
-    <row r="65" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -2982,7 +2985,7 @@
       <c r="AE65" s="6"/>
       <c r="AF65" s="6"/>
     </row>
-    <row r="66" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -3016,7 +3019,7 @@
       <c r="AE66" s="6"/>
       <c r="AF66" s="6"/>
     </row>
-    <row r="67" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -3050,7 +3053,7 @@
       <c r="AE67" s="6"/>
       <c r="AF67" s="6"/>
     </row>
-    <row r="68" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -3084,7 +3087,7 @@
       <c r="AE68" s="6"/>
       <c r="AF68" s="6"/>
     </row>
-    <row r="69" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -3118,7 +3121,7 @@
       <c r="AE69" s="6"/>
       <c r="AF69" s="6"/>
     </row>
-    <row r="70" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -3152,7 +3155,7 @@
       <c r="AE70" s="6"/>
       <c r="AF70" s="6"/>
     </row>
-    <row r="71" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -3186,7 +3189,7 @@
       <c r="AE71" s="6"/>
       <c r="AF71" s="6"/>
     </row>
-    <row r="72" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -3220,7 +3223,7 @@
       <c r="AE72" s="6"/>
       <c r="AF72" s="6"/>
     </row>
-    <row r="73" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -3254,7 +3257,7 @@
       <c r="AE73" s="6"/>
       <c r="AF73" s="6"/>
     </row>
-    <row r="74" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -3288,7 +3291,7 @@
       <c r="AE74" s="6"/>
       <c r="AF74" s="6"/>
     </row>
-    <row r="75" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -3322,7 +3325,7 @@
       <c r="AE75" s="6"/>
       <c r="AF75" s="6"/>
     </row>
-    <row r="76" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -3356,7 +3359,7 @@
       <c r="AE76" s="6"/>
       <c r="AF76" s="6"/>
     </row>
-    <row r="77" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -3390,7 +3393,7 @@
       <c r="AE77" s="6"/>
       <c r="AF77" s="6"/>
     </row>
-    <row r="78" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -3424,7 +3427,7 @@
       <c r="AE78" s="6"/>
       <c r="AF78" s="6"/>
     </row>
-    <row r="79" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
@@ -3458,7 +3461,7 @@
       <c r="AE79" s="6"/>
       <c r="AF79" s="6"/>
     </row>
-    <row r="80" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
@@ -3492,7 +3495,7 @@
       <c r="AE80" s="6"/>
       <c r="AF80" s="6"/>
     </row>
-    <row r="81" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
@@ -3526,7 +3529,7 @@
       <c r="AE81" s="6"/>
       <c r="AF81" s="6"/>
     </row>
-    <row r="82" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -3560,7 +3563,7 @@
       <c r="AE82" s="6"/>
       <c r="AF82" s="6"/>
     </row>
-    <row r="83" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -3594,7 +3597,7 @@
       <c r="AE83" s="6"/>
       <c r="AF83" s="6"/>
     </row>
-    <row r="84" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -3628,7 +3631,7 @@
       <c r="AE84" s="6"/>
       <c r="AF84" s="6"/>
     </row>
-    <row r="85" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -3662,7 +3665,7 @@
       <c r="AE85" s="6"/>
       <c r="AF85" s="6"/>
     </row>
-    <row r="86" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -3696,7 +3699,7 @@
       <c r="AE86" s="6"/>
       <c r="AF86" s="6"/>
     </row>
-    <row r="87" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -3730,7 +3733,7 @@
       <c r="AE87" s="6"/>
       <c r="AF87" s="6"/>
     </row>
-    <row r="88" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -3764,7 +3767,7 @@
       <c r="AE88" s="6"/>
       <c r="AF88" s="6"/>
     </row>
-    <row r="89" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -3798,7 +3801,7 @@
       <c r="AE89" s="6"/>
       <c r="AF89" s="6"/>
     </row>
-    <row r="90" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -3832,7 +3835,7 @@
       <c r="AE90" s="6"/>
       <c r="AF90" s="6"/>
     </row>
-    <row r="91" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -3866,7 +3869,7 @@
       <c r="AE91" s="6"/>
       <c r="AF91" s="6"/>
     </row>
-    <row r="92" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -3900,7 +3903,7 @@
       <c r="AE92" s="6"/>
       <c r="AF92" s="6"/>
     </row>
-    <row r="93" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -3934,7 +3937,7 @@
       <c r="AE93" s="6"/>
       <c r="AF93" s="6"/>
     </row>
-    <row r="94" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -3968,7 +3971,7 @@
       <c r="AE94" s="6"/>
       <c r="AF94" s="6"/>
     </row>
-    <row r="95" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -4002,7 +4005,7 @@
       <c r="AE95" s="6"/>
       <c r="AF95" s="6"/>
     </row>
-    <row r="96" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -4036,7 +4039,7 @@
       <c r="AE96" s="6"/>
       <c r="AF96" s="6"/>
     </row>
-    <row r="97" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
@@ -4070,7 +4073,7 @@
       <c r="AE97" s="6"/>
       <c r="AF97" s="6"/>
     </row>
-    <row r="98" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -4104,7 +4107,7 @@
       <c r="AE98" s="6"/>
       <c r="AF98" s="6"/>
     </row>
-    <row r="99" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6"/>
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
@@ -4138,7 +4141,7 @@
       <c r="AE99" s="6"/>
       <c r="AF99" s="6"/>
     </row>
-    <row r="100" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6"/>
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
@@ -4172,7 +4175,7 @@
       <c r="AE100" s="6"/>
       <c r="AF100" s="6"/>
     </row>
-    <row r="101" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6"/>
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
@@ -4206,7 +4209,7 @@
       <c r="AE101" s="6"/>
       <c r="AF101" s="6"/>
     </row>
-    <row r="102" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6"/>
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
@@ -4240,7 +4243,7 @@
       <c r="AE102" s="6"/>
       <c r="AF102" s="6"/>
     </row>
-    <row r="103" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6"/>
       <c r="B103" s="6"/>
       <c r="C103" s="6"/>
@@ -4274,7 +4277,7 @@
       <c r="AE103" s="6"/>
       <c r="AF103" s="6"/>
     </row>
-    <row r="104" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6"/>
       <c r="B104" s="6"/>
       <c r="C104" s="6"/>
@@ -4308,7 +4311,7 @@
       <c r="AE104" s="6"/>
       <c r="AF104" s="6"/>
     </row>
-    <row r="105" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6"/>
       <c r="B105" s="6"/>
       <c r="C105" s="6"/>
@@ -4342,7 +4345,7 @@
       <c r="AE105" s="6"/>
       <c r="AF105" s="6"/>
     </row>
-    <row r="106" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6"/>
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
@@ -4376,7 +4379,7 @@
       <c r="AE106" s="6"/>
       <c r="AF106" s="6"/>
     </row>
-    <row r="107" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6"/>
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
@@ -4410,7 +4413,7 @@
       <c r="AE107" s="6"/>
       <c r="AF107" s="6"/>
     </row>
-    <row r="108" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
@@ -4444,7 +4447,7 @@
       <c r="AE108" s="6"/>
       <c r="AF108" s="6"/>
     </row>
-    <row r="109" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
@@ -4478,7 +4481,7 @@
       <c r="AE109" s="6"/>
       <c r="AF109" s="6"/>
     </row>
-    <row r="110" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
@@ -4512,7 +4515,7 @@
       <c r="AE110" s="6"/>
       <c r="AF110" s="6"/>
     </row>
-    <row r="111" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6"/>
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
@@ -4546,7 +4549,7 @@
       <c r="AE111" s="6"/>
       <c r="AF111" s="6"/>
     </row>
-    <row r="112" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="6"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
@@ -4580,7 +4583,7 @@
       <c r="AE112" s="6"/>
       <c r="AF112" s="6"/>
     </row>
-    <row r="113" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
@@ -4614,7 +4617,7 @@
       <c r="AE113" s="6"/>
       <c r="AF113" s="6"/>
     </row>
-    <row r="114" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
@@ -4648,7 +4651,7 @@
       <c r="AE114" s="6"/>
       <c r="AF114" s="6"/>
     </row>
-    <row r="115" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
@@ -4682,7 +4685,7 @@
       <c r="AE115" s="6"/>
       <c r="AF115" s="6"/>
     </row>
-    <row r="116" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
@@ -4716,7 +4719,7 @@
       <c r="AE116" s="6"/>
       <c r="AF116" s="6"/>
     </row>
-    <row r="117" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
@@ -4750,7 +4753,7 @@
       <c r="AE117" s="6"/>
       <c r="AF117" s="6"/>
     </row>
-    <row r="118" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6"/>
       <c r="B118" s="6"/>
       <c r="C118" s="6"/>
@@ -4784,7 +4787,7 @@
       <c r="AE118" s="6"/>
       <c r="AF118" s="6"/>
     </row>
-    <row r="119" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="6"/>
       <c r="B119" s="6"/>
       <c r="C119" s="6"/>
@@ -4818,7 +4821,7 @@
       <c r="AE119" s="6"/>
       <c r="AF119" s="6"/>
     </row>
-    <row r="120" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
@@ -4852,7 +4855,7 @@
       <c r="AE120" s="6"/>
       <c r="AF120" s="6"/>
     </row>
-    <row r="121" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6"/>
       <c r="B121" s="6"/>
       <c r="C121" s="6"/>
@@ -4886,7 +4889,7 @@
       <c r="AE121" s="6"/>
       <c r="AF121" s="6"/>
     </row>
-    <row r="122" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6"/>
       <c r="B122" s="6"/>
       <c r="C122" s="6"/>
@@ -4920,7 +4923,7 @@
       <c r="AE122" s="6"/>
       <c r="AF122" s="6"/>
     </row>
-    <row r="123" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="6"/>
       <c r="B123" s="6"/>
       <c r="C123" s="6"/>
@@ -4954,7 +4957,7 @@
       <c r="AE123" s="6"/>
       <c r="AF123" s="6"/>
     </row>
-    <row r="124" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="6"/>
       <c r="B124" s="6"/>
       <c r="C124" s="6"/>
@@ -4988,7 +4991,7 @@
       <c r="AE124" s="6"/>
       <c r="AF124" s="6"/>
     </row>
-    <row r="125" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="6"/>
       <c r="B125" s="6"/>
       <c r="C125" s="6"/>
@@ -5022,7 +5025,7 @@
       <c r="AE125" s="6"/>
       <c r="AF125" s="6"/>
     </row>
-    <row r="126" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="6"/>
       <c r="B126" s="6"/>
       <c r="C126" s="6"/>
@@ -5056,7 +5059,7 @@
       <c r="AE126" s="6"/>
       <c r="AF126" s="6"/>
     </row>
-    <row r="127" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="6"/>
       <c r="B127" s="6"/>
       <c r="C127" s="6"/>
@@ -5090,7 +5093,7 @@
       <c r="AE127" s="6"/>
       <c r="AF127" s="6"/>
     </row>
-    <row r="128" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="6"/>
       <c r="B128" s="6"/>
       <c r="C128" s="6"/>
@@ -5124,7 +5127,7 @@
       <c r="AE128" s="6"/>
       <c r="AF128" s="6"/>
     </row>
-    <row r="129" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="6"/>
       <c r="B129" s="6"/>
       <c r="C129" s="6"/>
@@ -5158,7 +5161,7 @@
       <c r="AE129" s="6"/>
       <c r="AF129" s="6"/>
     </row>
-    <row r="130" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="6"/>
       <c r="B130" s="6"/>
       <c r="C130" s="6"/>
@@ -5192,7 +5195,7 @@
       <c r="AE130" s="6"/>
       <c r="AF130" s="6"/>
     </row>
-    <row r="131" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="6"/>
       <c r="B131" s="6"/>
       <c r="C131" s="6"/>
@@ -5226,7 +5229,7 @@
       <c r="AE131" s="6"/>
       <c r="AF131" s="6"/>
     </row>
-    <row r="132" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="6"/>
       <c r="B132" s="6"/>
       <c r="C132" s="6"/>
@@ -5260,7 +5263,7 @@
       <c r="AE132" s="6"/>
       <c r="AF132" s="6"/>
     </row>
-    <row r="133" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="6"/>
       <c r="B133" s="6"/>
       <c r="C133" s="6"/>
@@ -5294,7 +5297,7 @@
       <c r="AE133" s="6"/>
       <c r="AF133" s="6"/>
     </row>
-    <row r="134" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="6"/>
       <c r="B134" s="6"/>
       <c r="C134" s="6"/>
@@ -5328,7 +5331,7 @@
       <c r="AE134" s="6"/>
       <c r="AF134" s="6"/>
     </row>
-    <row r="135" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="6"/>
       <c r="B135" s="6"/>
       <c r="C135" s="6"/>
@@ -5362,7 +5365,7 @@
       <c r="AE135" s="6"/>
       <c r="AF135" s="6"/>
     </row>
-    <row r="136" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="6"/>
       <c r="B136" s="6"/>
       <c r="C136" s="6"/>
@@ -5396,7 +5399,7 @@
       <c r="AE136" s="6"/>
       <c r="AF136" s="6"/>
     </row>
-    <row r="137" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="6"/>
       <c r="B137" s="6"/>
       <c r="C137" s="6"/>
@@ -5430,7 +5433,7 @@
       <c r="AE137" s="6"/>
       <c r="AF137" s="6"/>
     </row>
-    <row r="138" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="6"/>
       <c r="B138" s="6"/>
       <c r="C138" s="6"/>
@@ -5464,7 +5467,7 @@
       <c r="AE138" s="6"/>
       <c r="AF138" s="6"/>
     </row>
-    <row r="139" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="6"/>
       <c r="B139" s="6"/>
       <c r="C139" s="6"/>
@@ -5498,7 +5501,7 @@
       <c r="AE139" s="6"/>
       <c r="AF139" s="6"/>
     </row>
-    <row r="140" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="6"/>
       <c r="B140" s="6"/>
       <c r="C140" s="6"/>
@@ -5532,7 +5535,7 @@
       <c r="AE140" s="6"/>
       <c r="AF140" s="6"/>
     </row>
-    <row r="141" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="6"/>
       <c r="B141" s="6"/>
       <c r="C141" s="6"/>
@@ -5566,7 +5569,7 @@
       <c r="AE141" s="6"/>
       <c r="AF141" s="6"/>
     </row>
-    <row r="142" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="6"/>
       <c r="B142" s="6"/>
       <c r="C142" s="6"/>
@@ -5600,7 +5603,7 @@
       <c r="AE142" s="6"/>
       <c r="AF142" s="6"/>
     </row>
-    <row r="143" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="6"/>
       <c r="B143" s="6"/>
       <c r="C143" s="6"/>
@@ -5634,7 +5637,7 @@
       <c r="AE143" s="6"/>
       <c r="AF143" s="6"/>
     </row>
-    <row r="144" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="6"/>
       <c r="B144" s="6"/>
       <c r="C144" s="6"/>
@@ -5668,7 +5671,7 @@
       <c r="AE144" s="6"/>
       <c r="AF144" s="6"/>
     </row>
-    <row r="145" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="6"/>
       <c r="B145" s="6"/>
       <c r="C145" s="6"/>
@@ -5702,7 +5705,7 @@
       <c r="AE145" s="6"/>
       <c r="AF145" s="6"/>
     </row>
-    <row r="146" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="6"/>
       <c r="B146" s="6"/>
       <c r="C146" s="6"/>
@@ -5736,7 +5739,7 @@
       <c r="AE146" s="6"/>
       <c r="AF146" s="6"/>
     </row>
-    <row r="147" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="6"/>
       <c r="B147" s="6"/>
       <c r="C147" s="6"/>
@@ -5770,7 +5773,7 @@
       <c r="AE147" s="6"/>
       <c r="AF147" s="6"/>
     </row>
-    <row r="148" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="6"/>
       <c r="B148" s="6"/>
       <c r="C148" s="6"/>
@@ -5804,7 +5807,7 @@
       <c r="AE148" s="6"/>
       <c r="AF148" s="6"/>
     </row>
-    <row r="149" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="6"/>
       <c r="B149" s="6"/>
       <c r="C149" s="6"/>
@@ -5838,7 +5841,7 @@
       <c r="AE149" s="6"/>
       <c r="AF149" s="6"/>
     </row>
-    <row r="150" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="6"/>
       <c r="B150" s="6"/>
       <c r="C150" s="6"/>
@@ -5872,7 +5875,7 @@
       <c r="AE150" s="6"/>
       <c r="AF150" s="6"/>
     </row>
-    <row r="151" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="6"/>
       <c r="B151" s="6"/>
       <c r="C151" s="6"/>
@@ -5906,7 +5909,7 @@
       <c r="AE151" s="6"/>
       <c r="AF151" s="6"/>
     </row>
-    <row r="152" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="6"/>
       <c r="B152" s="6"/>
       <c r="C152" s="6"/>
@@ -5940,7 +5943,7 @@
       <c r="AE152" s="6"/>
       <c r="AF152" s="6"/>
     </row>
-    <row r="153" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="6"/>
       <c r="B153" s="6"/>
       <c r="C153" s="6"/>
@@ -5974,7 +5977,7 @@
       <c r="AE153" s="6"/>
       <c r="AF153" s="6"/>
     </row>
-    <row r="154" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="6"/>
       <c r="B154" s="6"/>
       <c r="C154" s="6"/>
@@ -6008,7 +6011,7 @@
       <c r="AE154" s="6"/>
       <c r="AF154" s="6"/>
     </row>
-    <row r="155" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="6"/>
       <c r="B155" s="6"/>
       <c r="C155" s="6"/>
@@ -6042,7 +6045,7 @@
       <c r="AE155" s="6"/>
       <c r="AF155" s="6"/>
     </row>
-    <row r="156" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="6"/>
       <c r="B156" s="6"/>
       <c r="C156" s="6"/>
@@ -6076,7 +6079,7 @@
       <c r="AE156" s="6"/>
       <c r="AF156" s="6"/>
     </row>
-    <row r="157" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="6"/>
       <c r="B157" s="6"/>
       <c r="C157" s="6"/>
@@ -6110,7 +6113,7 @@
       <c r="AE157" s="6"/>
       <c r="AF157" s="6"/>
     </row>
-    <row r="158" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="6"/>
       <c r="B158" s="6"/>
       <c r="C158" s="6"/>
@@ -6144,7 +6147,7 @@
       <c r="AE158" s="6"/>
       <c r="AF158" s="6"/>
     </row>
-    <row r="159" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="6"/>
       <c r="B159" s="6"/>
       <c r="C159" s="6"/>
@@ -6178,7 +6181,7 @@
       <c r="AE159" s="6"/>
       <c r="AF159" s="6"/>
     </row>
-    <row r="160" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="6"/>
       <c r="B160" s="6"/>
       <c r="C160" s="6"/>
@@ -6212,7 +6215,7 @@
       <c r="AE160" s="6"/>
       <c r="AF160" s="6"/>
     </row>
-    <row r="161" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="6"/>
       <c r="B161" s="6"/>
       <c r="C161" s="6"/>
@@ -6246,7 +6249,7 @@
       <c r="AE161" s="6"/>
       <c r="AF161" s="6"/>
     </row>
-    <row r="162" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="6"/>
       <c r="B162" s="6"/>
       <c r="C162" s="6"/>
@@ -6280,7 +6283,7 @@
       <c r="AE162" s="6"/>
       <c r="AF162" s="6"/>
     </row>
-    <row r="163" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="6"/>
       <c r="B163" s="6"/>
       <c r="C163" s="6"/>
@@ -6314,7 +6317,7 @@
       <c r="AE163" s="6"/>
       <c r="AF163" s="6"/>
     </row>
-    <row r="164" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="6"/>
       <c r="B164" s="6"/>
       <c r="C164" s="6"/>
@@ -6348,7 +6351,7 @@
       <c r="AE164" s="6"/>
       <c r="AF164" s="6"/>
     </row>
-    <row r="165" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="6"/>
       <c r="B165" s="6"/>
       <c r="C165" s="6"/>
@@ -6382,7 +6385,7 @@
       <c r="AE165" s="6"/>
       <c r="AF165" s="6"/>
     </row>
-    <row r="166" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="6"/>
       <c r="B166" s="6"/>
       <c r="C166" s="6"/>
@@ -6416,7 +6419,7 @@
       <c r="AE166" s="6"/>
       <c r="AF166" s="6"/>
     </row>
-    <row r="167" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="6"/>
       <c r="B167" s="6"/>
       <c r="C167" s="6"/>
@@ -6450,7 +6453,7 @@
       <c r="AE167" s="6"/>
       <c r="AF167" s="6"/>
     </row>
-    <row r="168" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="6"/>
       <c r="B168" s="6"/>
       <c r="C168" s="6"/>
@@ -6484,7 +6487,7 @@
       <c r="AE168" s="6"/>
       <c r="AF168" s="6"/>
     </row>
-    <row r="169" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="6"/>
       <c r="B169" s="6"/>
       <c r="C169" s="6"/>
@@ -6518,7 +6521,7 @@
       <c r="AE169" s="6"/>
       <c r="AF169" s="6"/>
     </row>
-    <row r="170" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="6"/>
       <c r="B170" s="6"/>
       <c r="C170" s="6"/>
@@ -6552,7 +6555,7 @@
       <c r="AE170" s="6"/>
       <c r="AF170" s="6"/>
     </row>
-    <row r="171" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="6"/>
       <c r="B171" s="6"/>
       <c r="C171" s="6"/>
@@ -6586,7 +6589,7 @@
       <c r="AE171" s="6"/>
       <c r="AF171" s="6"/>
     </row>
-    <row r="172" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="6"/>
       <c r="B172" s="6"/>
       <c r="C172" s="6"/>
@@ -6620,7 +6623,7 @@
       <c r="AE172" s="6"/>
       <c r="AF172" s="6"/>
     </row>
-    <row r="173" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="6"/>
       <c r="B173" s="6"/>
       <c r="C173" s="6"/>
@@ -6654,7 +6657,7 @@
       <c r="AE173" s="6"/>
       <c r="AF173" s="6"/>
     </row>
-    <row r="174" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="6"/>
       <c r="B174" s="6"/>
       <c r="C174" s="6"/>
@@ -6688,7 +6691,7 @@
       <c r="AE174" s="6"/>
       <c r="AF174" s="6"/>
     </row>
-    <row r="175" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="6"/>
       <c r="B175" s="6"/>
       <c r="C175" s="6"/>
@@ -6722,7 +6725,7 @@
       <c r="AE175" s="6"/>
       <c r="AF175" s="6"/>
     </row>
-    <row r="176" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="6"/>
       <c r="B176" s="6"/>
       <c r="C176" s="6"/>
@@ -6756,7 +6759,7 @@
       <c r="AE176" s="6"/>
       <c r="AF176" s="6"/>
     </row>
-    <row r="177" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="6"/>
       <c r="B177" s="6"/>
       <c r="C177" s="6"/>
@@ -6790,7 +6793,7 @@
       <c r="AE177" s="6"/>
       <c r="AF177" s="6"/>
     </row>
-    <row r="178" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="6"/>
       <c r="B178" s="6"/>
       <c r="C178" s="6"/>
@@ -6824,7 +6827,7 @@
       <c r="AE178" s="6"/>
       <c r="AF178" s="6"/>
     </row>
-    <row r="179" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="6"/>
       <c r="B179" s="6"/>
       <c r="C179" s="6"/>
@@ -6858,7 +6861,7 @@
       <c r="AE179" s="6"/>
       <c r="AF179" s="6"/>
     </row>
-    <row r="180" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="6"/>
       <c r="B180" s="6"/>
       <c r="C180" s="6"/>
@@ -6892,7 +6895,7 @@
       <c r="AE180" s="6"/>
       <c r="AF180" s="6"/>
     </row>
-    <row r="181" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="6"/>
       <c r="B181" s="6"/>
       <c r="C181" s="6"/>
@@ -6926,7 +6929,7 @@
       <c r="AE181" s="6"/>
       <c r="AF181" s="6"/>
     </row>
-    <row r="182" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="6"/>
       <c r="B182" s="6"/>
       <c r="C182" s="6"/>
@@ -6960,7 +6963,7 @@
       <c r="AE182" s="6"/>
       <c r="AF182" s="6"/>
     </row>
-    <row r="183" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="6"/>
       <c r="B183" s="6"/>
       <c r="C183" s="6"/>
@@ -6994,7 +6997,7 @@
       <c r="AE183" s="6"/>
       <c r="AF183" s="6"/>
     </row>
-    <row r="184" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="6"/>
       <c r="B184" s="6"/>
       <c r="C184" s="6"/>
@@ -7028,7 +7031,7 @@
       <c r="AE184" s="6"/>
       <c r="AF184" s="6"/>
     </row>
-    <row r="185" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="6"/>
       <c r="B185" s="6"/>
       <c r="C185" s="6"/>
@@ -7062,7 +7065,7 @@
       <c r="AE185" s="6"/>
       <c r="AF185" s="6"/>
     </row>
-    <row r="186" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="6"/>
       <c r="B186" s="6"/>
       <c r="C186" s="6"/>
@@ -7096,7 +7099,7 @@
       <c r="AE186" s="6"/>
       <c r="AF186" s="6"/>
     </row>
-    <row r="187" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="6"/>
       <c r="B187" s="6"/>
       <c r="C187" s="6"/>
@@ -7130,7 +7133,7 @@
       <c r="AE187" s="6"/>
       <c r="AF187" s="6"/>
     </row>
-    <row r="188" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="6"/>
       <c r="B188" s="6"/>
       <c r="C188" s="6"/>
@@ -7164,7 +7167,7 @@
       <c r="AE188" s="6"/>
       <c r="AF188" s="6"/>
     </row>
-    <row r="189" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="6"/>
       <c r="B189" s="6"/>
       <c r="C189" s="6"/>
@@ -7198,7 +7201,7 @@
       <c r="AE189" s="6"/>
       <c r="AF189" s="6"/>
     </row>
-    <row r="190" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="6"/>
       <c r="B190" s="6"/>
       <c r="C190" s="6"/>
@@ -7232,7 +7235,7 @@
       <c r="AE190" s="6"/>
       <c r="AF190" s="6"/>
     </row>
-    <row r="191" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="6"/>
       <c r="B191" s="6"/>
       <c r="C191" s="6"/>
@@ -7266,7 +7269,7 @@
       <c r="AE191" s="6"/>
       <c r="AF191" s="6"/>
     </row>
-    <row r="192" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="6"/>
       <c r="B192" s="6"/>
       <c r="C192" s="6"/>
@@ -7300,7 +7303,7 @@
       <c r="AE192" s="6"/>
       <c r="AF192" s="6"/>
     </row>
-    <row r="193" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="6"/>
       <c r="B193" s="6"/>
       <c r="C193" s="6"/>
@@ -7334,7 +7337,7 @@
       <c r="AE193" s="6"/>
       <c r="AF193" s="6"/>
     </row>
-    <row r="194" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="6"/>
       <c r="B194" s="6"/>
       <c r="C194" s="6"/>
@@ -7368,7 +7371,7 @@
       <c r="AE194" s="6"/>
       <c r="AF194" s="6"/>
     </row>
-    <row r="195" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="6"/>
       <c r="B195" s="6"/>
       <c r="C195" s="6"/>
@@ -7402,7 +7405,7 @@
       <c r="AE195" s="6"/>
       <c r="AF195" s="6"/>
     </row>
-    <row r="196" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="6"/>
       <c r="B196" s="6"/>
       <c r="C196" s="6"/>
@@ -7436,7 +7439,7 @@
       <c r="AE196" s="6"/>
       <c r="AF196" s="6"/>
     </row>
-    <row r="197" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="6"/>
       <c r="B197" s="6"/>
       <c r="C197" s="6"/>
@@ -7470,7 +7473,7 @@
       <c r="AE197" s="6"/>
       <c r="AF197" s="6"/>
     </row>
-    <row r="198" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="6"/>
       <c r="B198" s="6"/>
       <c r="C198" s="6"/>
@@ -7504,7 +7507,7 @@
       <c r="AE198" s="6"/>
       <c r="AF198" s="6"/>
     </row>
-    <row r="199" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="6"/>
       <c r="B199" s="6"/>
       <c r="C199" s="6"/>
@@ -7538,7 +7541,7 @@
       <c r="AE199" s="6"/>
       <c r="AF199" s="6"/>
     </row>
-    <row r="200" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="6"/>
       <c r="B200" s="6"/>
       <c r="C200" s="6"/>
@@ -7572,7 +7575,7 @@
       <c r="AE200" s="6"/>
       <c r="AF200" s="6"/>
     </row>
-    <row r="201" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="6"/>
       <c r="B201" s="6"/>
       <c r="C201" s="6"/>
@@ -7606,7 +7609,7 @@
       <c r="AE201" s="6"/>
       <c r="AF201" s="6"/>
     </row>
-    <row r="202" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:32" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="6"/>
       <c r="B202" s="6"/>
       <c r="C202" s="6"/>
@@ -7640,789 +7643,789 @@
       <c r="AE202" s="6"/>
       <c r="AF202" s="6"/>
     </row>
-    <row r="203" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="204" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="205" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="206" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="207" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="208" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P3" r:id="rId1"/>
+    <hyperlink ref="P3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId2"/>

</xml_diff>